<commit_message>
improve consistency of labels in KDF
</commit_message>
<xml_diff>
--- a/masterlist.xlsx
+++ b/masterlist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="171">
   <si>
     <t xml:space="preserve">Klasse</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
+    <t xml:space="preserve">Notizen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ausgruendung</t>
   </si>
   <si>
@@ -196,6 +199,9 @@
     <t xml:space="preserve">Patent</t>
   </si>
   <si>
+    <t xml:space="preserve">nicht relevant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Person</t>
   </si>
   <si>
@@ -422,6 +428,9 @@
   </si>
   <si>
     <t xml:space="preserve">hatAnmelder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bezieht sich nur auf Patente</t>
   </si>
   <si>
     <t xml:space="preserve">hatArt</t>
@@ -647,18 +656,18 @@
   </sheetPr>
   <dimension ref="A1:M160"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A133" activeCellId="0" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.7755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,7 +686,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -688,10 +699,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>0</v>
@@ -700,15 +711,15 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>0</v>
@@ -717,32 +728,32 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>0</v>
@@ -751,15 +762,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>0</v>
@@ -768,15 +779,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>0</v>
@@ -785,16 +796,16 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="0" t="s">
         <v>0</v>
       </c>
@@ -802,15 +813,15 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>0</v>
@@ -819,15 +830,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>0</v>
@@ -836,15 +847,15 @@
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>0</v>
@@ -853,15 +864,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>0</v>
@@ -870,15 +881,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>0</v>
@@ -887,15 +898,15 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>0</v>
@@ -904,15 +915,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>0</v>
@@ -921,15 +932,15 @@
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>0</v>
@@ -938,15 +949,15 @@
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>0</v>
@@ -955,15 +966,15 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>0</v>
@@ -972,16 +983,16 @@
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="C19" s="0" t="s">
         <v>0</v>
       </c>
@@ -989,15 +1000,15 @@
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>0</v>
@@ -1006,15 +1017,15 @@
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>0</v>
@@ -1023,15 +1034,15 @@
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>0</v>
@@ -1040,15 +1051,15 @@
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>0</v>
@@ -1057,15 +1068,15 @@
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>0</v>
@@ -1074,15 +1085,15 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>0</v>
@@ -1091,15 +1102,15 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>0</v>
@@ -1108,16 +1119,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="C27" s="0" t="s">
         <v>0</v>
       </c>
@@ -1125,15 +1136,15 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>0</v>
@@ -1142,15 +1153,15 @@
         <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>0</v>
@@ -1159,15 +1170,15 @@
         <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>0</v>
@@ -1176,16 +1187,16 @@
         <v>1</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="C31" s="0" t="s">
         <v>0</v>
       </c>
@@ -1193,15 +1204,15 @@
         <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>0</v>
@@ -1210,15 +1221,15 @@
         <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>0</v>
@@ -1227,15 +1238,15 @@
         <v>1</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>0</v>
@@ -1244,15 +1255,15 @@
         <v>1</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>0</v>
@@ -1261,15 +1272,15 @@
         <v>1</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>0</v>
@@ -1278,15 +1289,15 @@
         <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>0</v>
@@ -1295,16 +1306,16 @@
         <v>1</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="C38" s="0" t="s">
         <v>0</v>
       </c>
@@ -1312,15 +1323,15 @@
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>0</v>
@@ -1329,15 +1340,15 @@
         <v>1</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>0</v>
@@ -1346,15 +1357,15 @@
         <v>1</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>0</v>
@@ -1363,16 +1374,16 @@
         <v>1</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="C42" s="0" t="s">
         <v>0</v>
       </c>
@@ -1380,15 +1391,15 @@
         <v>1</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>0</v>
@@ -1397,15 +1408,15 @@
         <v>1</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>0</v>
@@ -1414,15 +1425,15 @@
         <v>1</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>0</v>
@@ -1431,16 +1442,16 @@
         <v>1</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="C46" s="0" t="s">
         <v>0</v>
       </c>
@@ -1448,15 +1459,15 @@
         <v>1</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>0</v>
@@ -1465,15 +1476,15 @@
         <v>1</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>0</v>
@@ -1482,15 +1493,15 @@
         <v>1</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>0</v>
@@ -1499,15 +1510,15 @@
         <v>1</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>0</v>
@@ -1516,15 +1527,15 @@
         <v>1</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>0</v>
@@ -1533,15 +1544,18 @@
         <v>1</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>0</v>
@@ -1550,15 +1564,15 @@
         <v>1</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>0</v>
@@ -1567,15 +1581,15 @@
         <v>1</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>0</v>
@@ -1584,15 +1598,15 @@
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>0</v>
@@ -1601,16 +1615,16 @@
         <v>1</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="C56" s="0" t="s">
         <v>0</v>
       </c>
@@ -1618,15 +1632,15 @@
         <v>1</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>0</v>
@@ -1635,15 +1649,15 @@
         <v>1</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>0</v>
@@ -1652,16 +1666,16 @@
         <v>1</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="C59" s="0" t="s">
         <v>0</v>
       </c>
@@ -1669,15 +1683,15 @@
         <v>1</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>0</v>
@@ -1686,15 +1700,15 @@
         <v>1</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>0</v>
@@ -1703,15 +1717,15 @@
         <v>1</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>0</v>
@@ -1720,15 +1734,15 @@
         <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>0</v>
@@ -1737,15 +1751,15 @@
         <v>1</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>0</v>
@@ -1754,16 +1768,16 @@
         <v>1</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="C65" s="0" t="s">
         <v>0</v>
       </c>
@@ -1771,15 +1785,15 @@
         <v>1</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>0</v>
@@ -1788,16 +1802,16 @@
         <v>1</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="C67" s="0" t="s">
         <v>0</v>
       </c>
@@ -1805,15 +1819,15 @@
         <v>1</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>0</v>
@@ -1822,15 +1836,15 @@
         <v>1</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>0</v>
@@ -1839,15 +1853,15 @@
         <v>1</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>0</v>
@@ -1856,15 +1870,15 @@
         <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>0</v>
@@ -1873,15 +1887,15 @@
         <v>1</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>0</v>
@@ -1890,15 +1904,15 @@
         <v>1</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>0</v>
@@ -1907,16 +1921,16 @@
         <v>1</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="C74" s="0" t="s">
         <v>0</v>
       </c>
@@ -1924,15 +1938,15 @@
         <v>1</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>0</v>
@@ -1941,15 +1955,15 @@
         <v>1</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>0</v>
@@ -1958,15 +1972,15 @@
         <v>1</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>0</v>
@@ -1975,15 +1989,15 @@
         <v>1</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>0</v>
@@ -1992,15 +2006,15 @@
         <v>1</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>0</v>
@@ -2009,16 +2023,16 @@
         <v>1</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="C80" s="0" t="s">
         <v>0</v>
       </c>
@@ -2026,15 +2040,15 @@
         <v>1</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>0</v>
@@ -2043,16 +2057,16 @@
         <v>1</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="C82" s="0" t="s">
         <v>0</v>
       </c>
@@ -2060,15 +2074,15 @@
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>0</v>
@@ -2077,15 +2091,15 @@
         <v>1</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>0</v>
@@ -2094,15 +2108,15 @@
         <v>1</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>0</v>
@@ -2111,15 +2125,15 @@
         <v>1</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>0</v>
@@ -2128,16 +2142,16 @@
         <v>1</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>91</v>
-      </c>
       <c r="C87" s="0" t="s">
         <v>0</v>
       </c>
@@ -2145,15 +2159,15 @@
         <v>1</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>0</v>
@@ -2162,15 +2176,15 @@
         <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>0</v>
@@ -2179,15 +2193,15 @@
         <v>1</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>0</v>
@@ -2196,15 +2210,15 @@
         <v>1</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>0</v>
@@ -2213,15 +2227,15 @@
         <v>1</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>0</v>
@@ -2230,15 +2244,15 @@
         <v>1</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>0</v>
@@ -2247,15 +2261,15 @@
         <v>1</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>0</v>
@@ -2264,15 +2278,15 @@
         <v>1</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>0</v>
@@ -2281,15 +2295,15 @@
         <v>1</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>0</v>
@@ -2298,16 +2312,16 @@
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B97" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="C97" s="0" t="s">
         <v>0</v>
       </c>
@@ -2315,15 +2329,15 @@
         <v>1</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>0</v>
@@ -2332,15 +2346,15 @@
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>0</v>
@@ -2349,15 +2363,15 @@
         <v>1</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>0</v>
@@ -2366,15 +2380,15 @@
         <v>1</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>0</v>
@@ -2383,16 +2397,16 @@
         <v>1</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B102" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="C102" s="0" t="s">
         <v>0</v>
       </c>
@@ -2400,15 +2414,15 @@
         <v>1</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>0</v>
@@ -2417,15 +2431,15 @@
         <v>1</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>0</v>
@@ -2434,16 +2448,16 @@
         <v>1</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B105" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="C105" s="0" t="s">
         <v>0</v>
       </c>
@@ -2451,15 +2465,15 @@
         <v>1</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>0</v>
@@ -2468,15 +2482,15 @@
         <v>1</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>0</v>
@@ -2485,15 +2499,15 @@
         <v>1</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>0</v>
@@ -2502,16 +2516,16 @@
         <v>1</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B109" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B109" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="C109" s="0" t="s">
         <v>0</v>
       </c>
@@ -2519,15 +2533,15 @@
         <v>1</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>0</v>
@@ -2536,15 +2550,15 @@
         <v>1</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>0</v>
@@ -2553,15 +2567,15 @@
         <v>1</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>0</v>
@@ -2570,15 +2584,15 @@
         <v>1</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>0</v>
@@ -2587,15 +2601,15 @@
         <v>1</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>0</v>
@@ -2604,15 +2618,15 @@
         <v>1</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>0</v>
@@ -2621,15 +2635,15 @@
         <v>1</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>0</v>
@@ -2638,15 +2652,15 @@
         <v>1</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>0</v>
@@ -2655,16 +2669,16 @@
         <v>1</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B118" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B118" s="0" t="s">
-        <v>122</v>
-      </c>
       <c r="C118" s="0" t="s">
         <v>0</v>
       </c>
@@ -2672,15 +2686,15 @@
         <v>1</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>0</v>
@@ -2689,15 +2703,15 @@
         <v>1</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>0</v>
@@ -2706,15 +2720,15 @@
         <v>1</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>0</v>
@@ -2723,15 +2737,15 @@
         <v>1</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C122" s="0" t="s">
         <v>0</v>
@@ -2740,16 +2754,16 @@
         <v>1</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B123" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B123" s="0" t="s">
-        <v>127</v>
-      </c>
       <c r="C123" s="0" t="s">
         <v>0</v>
       </c>
@@ -2757,15 +2771,15 @@
         <v>1</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>0</v>
@@ -2774,619 +2788,622 @@
         <v>1</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D125" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="F126" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D127" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D128" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D129" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D131" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D132" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D133" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D134" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D135" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D136" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D137" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D140" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D141" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D143" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D144" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D145" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D146" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D148" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D149" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D150" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D151" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D152" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D153" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D155" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D160" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>